<commit_message>
fix RO checker of qty
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA13D90-7774-4892-8276-88062BC4B3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="30465" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -216,51 +217,63 @@
     <t>Scope of Work</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>Testing Purpose</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply of labor ~Relay on SSR 125 AVR~Scope of works:~1. Testing1~2. Testing2 </t>
-  </si>
-  <si>
-    <t>PPE~Manpower~Scope of works:~1.Trial1~2.Trial2</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>1.Note2</t>
-  </si>
-  <si>
-    <t>2.Note3</t>
-  </si>
-  <si>
-    <t>3.Note4</t>
-  </si>
-  <si>
-    <t>4.Note5</t>
-  </si>
-  <si>
-    <t>PPE1~Manpower2~Scope of works:~1.Trial12~2.Trial23</t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>JO2021-01</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen ~ Relay on SSR125 AVR at DG 4 &amp; DG 5. ~ Scope of works include but not limited to the following: ~ 1. Wiring of Signal from EasyGen to AVR ~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load  step response. ~ 3. Simulation and Functional Test.</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t>Tools and Equipment: List of tools and equipment</t>
+  </si>
+  <si>
+    <t>Mobilization: Inform CENPRI of mobilization 2 days prior start of project</t>
+  </si>
+  <si>
+    <t>Duration: Contractor to submit gantt chart before the start of work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warranty: Contractor to include in quotation </t>
+  </si>
+  <si>
+    <t>Service Report: Submission of service report right after completion of the scope of work</t>
+  </si>
+  <si>
+    <t>Demobilization: Secure housekeeping and gate pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
+  </si>
+  <si>
+    <t>lots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +320,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +368,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -448,11 +501,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,21 +715,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,18 +730,33 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,42 +766,106 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{43C452A1-B806-4B5F-A581-94827FACDBCC}"/>
+    <cellStyle name="Normal 5 2" xfId="2" xr:uid="{EBD4F205-B19E-4952-83C3-683979B80B68}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,7 +906,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -887,11 +1203,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,14 +1237,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -936,14 +1252,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -951,14 +1267,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -966,148 +1282,144 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="23">
-        <v>5</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="29"/>
+      <c r="I7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="26">
-        <v>44270</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="27">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="39">
-        <v>44271</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="29"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="32">
-        <v>44272</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="29"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="29"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="23">
-        <v>1</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="29"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="29"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="19"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1117,175 +1429,216 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="13">
+      <c r="B14" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="53">
+        <v>1</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>1</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
         <v>2</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="10">
-        <v>100</v>
-      </c>
-      <c r="J14" s="20">
-        <v>200</v>
-      </c>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="13">
+      <c r="B19" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
         <v>3</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="10">
-        <v>200</v>
-      </c>
-      <c r="J15" s="20">
-        <v>600</v>
-      </c>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="23" t="s">
+      <c r="B20" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>4</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>5</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>6</v>
+      </c>
+      <c r="B23" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="13">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="10">
-        <v>500</v>
-      </c>
-      <c r="J16" s="20">
-        <v>500</v>
-      </c>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="29"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="29"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="29"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+    </row>
+    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>7</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>8</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="52"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
+  <mergeCells count="41">
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
@@ -1302,15 +1655,18 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1319,7 +1675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fixed Display Jo No
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -216,40 +216,31 @@
     <t>Scope of Work</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>Testing Purpose</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply of labor ~Relay on SSR 125 AVR~Scope of works:~1. Testing1~2. Testing2 </t>
-  </si>
-  <si>
-    <t>PPE~Manpower~Scope of works:~1.Trial1~2.Trial2</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>1.Note2</t>
-  </si>
-  <si>
-    <t>2.Note3</t>
-  </si>
-  <si>
-    <t>3.Note4</t>
-  </si>
-  <si>
-    <t>4.Note5</t>
-  </si>
-  <si>
-    <t>PPE1~Manpower2~Scope of works:~1.Trial12~2.Trial23</t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen ~ Relay on SSR125 AVR at DG 4 &amp; DG 5. ~ Scope of works include but not limited to the following: ~ 1. Wiring of Signal from EasyGen to AVR ~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load  step response. ~ 3. Simulation and Functional Test.</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>JO2022-03</t>
   </si>
 </sst>
 </file>
@@ -260,7 +251,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +298,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +346,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -448,11 +479,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,8 +693,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,27 +804,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,18 +818,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,8 +840,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,7 +884,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -888,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,14 +1215,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -936,14 +1230,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -951,14 +1245,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -966,148 +1260,142 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="42"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="23">
-        <v>5</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="29"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="42"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="26">
-        <v>44270</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="53">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="39">
-        <v>44271</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="29"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="42"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="32">
-        <v>44272</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="29"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="42"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="29"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="E10" s="42"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="23">
-        <v>1</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="29"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="42"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="29"/>
+      <c r="C11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="42"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="19"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1117,177 +1405,181 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="13">
-        <v>2</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="10">
-        <v>100</v>
-      </c>
-      <c r="J14" s="20">
-        <v>200</v>
-      </c>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="23" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="13">
-        <v>3</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="10">
-        <v>200</v>
-      </c>
-      <c r="J15" s="20">
-        <v>600</v>
-      </c>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="13">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="10">
-        <v>500</v>
-      </c>
-      <c r="J16" s="20">
-        <v>500</v>
-      </c>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="29"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="29"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="29"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="41">
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1298,19 +1590,31 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add functionality in jorfq list
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -217,30 +217,6 @@
   </si>
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>Bacolod Office</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>IT Office Renovation</t>
-  </si>
-  <si>
-    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen ~ Relay on SSR125 AVR at DG 4 &amp; DG 5. ~ Scope of works include but not limited to the following: ~ 1. Wiring of Signal from EasyGen to AVR ~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load  step response. ~ 3. Simulation and Functional Test.</t>
-  </si>
-  <si>
-    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
-  </si>
-  <si>
-    <t>lots</t>
-  </si>
-  <si>
-    <t>JO2022-03</t>
   </si>
 </sst>
 </file>
@@ -251,7 +227,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,36 +274,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,20 +294,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -479,203 +415,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,52 +437,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,55 +463,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -818,6 +481,18 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -840,10 +515,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
-    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -884,7 +557,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1182,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="C11" sqref="C11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,14 +888,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -1230,14 +903,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -1245,14 +918,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -1260,142 +933,132 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="42"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="29"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="42"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="53">
-        <v>44273</v>
-      </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="42"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="42"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="29"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="42"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="42"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1405,181 +1068,133 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="26">
-        <v>1</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>70</v>
-      </c>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="37">
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1590,31 +1205,19 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C12:K12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updates in jo rfq
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,43 +219,28 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen ~ Relay on SSR125 AVR at DG 4 &amp; DG 5. ~ Scope of works include but not limited to the following: ~ 1. Wiring of Signal from EasyGen to AVR ~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load  step response. ~ 3. Simulation and Functional Test.</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
   </si>
   <si>
     <t>lots</t>
   </si>
   <si>
-    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing before conducting first day of work.      </t>
-  </si>
-  <si>
-    <t>Tools and Equipment: List of tools and equipment</t>
-  </si>
-  <si>
-    <t>Mobilization: Inform CENPRI of mobilization 2 days prior start of project</t>
-  </si>
-  <si>
-    <t>Duration: Contractor to submit gantt chart before the start of work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warranty: Contractor to include in quotation </t>
-  </si>
-  <si>
-    <t>Service Report: Submission of service report right after completion of the scope of work</t>
-  </si>
-  <si>
-    <t>Demobilization: Secure housekeeping and gate pass</t>
-  </si>
-  <si>
-    <t>CENJO-EM005-21</t>
-  </si>
-  <si>
-    <t>For Grid Compliance Re-Testing with NGCP on DG 1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 5. ~Scope of works include but not limited to the following: ~1. Wiring of Signal from EasyGen to AVR ~2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response. ~3. Simulation and Functional Test.           </t>
+    <t>JO2022-03</t>
   </si>
 </sst>
 </file>
@@ -266,7 +251,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,14 +284,50 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,8 +346,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -446,11 +479,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -468,113 +693,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -606,7 +875,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -913,25 +1182,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -944,194 +1212,190 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="52"/>
+      <c r="C7" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="42"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="I7" s="41"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="42"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="28">
-        <v>44229</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="53">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="28">
-        <v>44229</v>
-      </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="I8" s="62"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="42"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="28">
-        <v>44229</v>
-      </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="I9" s="48"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="42"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="E10" s="42"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I10" s="41"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="42"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="42"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1141,205 +1405,181 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="36"/>
-    </row>
-    <row r="14" spans="1:15" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="42">
+      <c r="B14" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="26">
         <v>1</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="39">
-        <v>200</v>
-      </c>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H14" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="45" t="s">
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="17"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
+  <mergeCells count="41">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1350,22 +1590,31 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1378,7 +1627,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add function to JOI
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,34 +219,37 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Bacolod Office</t>
+    <t>Requested By:</t>
+  </si>
+  <si>
+    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 5.~ Scope of works include but not limited to the following:~ 1. Wiring of Signal from EasyGen to AVR~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response.~ 3. Simulation and Functional Test.</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 51.~ Scope of works include but not limited to the following1:~ 1. Wiring of Signal from EasyGen to AVR1~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response1.~ 3. Simulation and Functional Test1.</t>
+  </si>
+  <si>
+    <t>Bacolod</t>
   </si>
   <si>
     <t>IT</t>
   </si>
   <si>
-    <t>IT Office Renovation</t>
-  </si>
-  <si>
-    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen ~ Relay on SSR125 AVR at DG 4 &amp; DG 5. ~ Scope of works include but not limited to the following: ~ 1. Wiring of Signal from EasyGen to AVR ~ 2. Configuration of EasyGen relay for excitation of On-Load and Off-Load  step response. ~ 3. Simulation and Functional Test.</t>
-  </si>
-  <si>
-    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
-  </si>
-  <si>
-    <t>lots</t>
-  </si>
-  <si>
-    <t>JO2022-03</t>
-  </si>
-  <si>
-    <t>Sample 1</t>
-  </si>
-  <si>
-    <t>Sample 2</t>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
+    <t>Testing only</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,36 +307,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,20 +327,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -485,203 +448,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,57 +470,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -758,63 +487,33 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,32 +523,36 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
-    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1188,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:F21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,14 +924,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -1236,14 +939,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -1251,14 +954,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -1266,142 +969,152 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="42"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="42"/>
+      <c r="I7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="53">
-        <v>44273</v>
-      </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="29">
+        <v>44284</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="42"/>
+      <c r="I8" s="28">
+        <v>44286</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="42"/>
+      <c r="I9" s="32">
+        <v>44291</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="42"/>
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="42"/>
+      <c r="A11" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1411,185 +1124,162 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="37"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="26">
+      <c r="B14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13">
         <v>1</v>
       </c>
-      <c r="H14" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="H14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="10">
+        <v>100</v>
+      </c>
+      <c r="J14" s="18">
+        <v>100</v>
+      </c>
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="13">
+        <v>2</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="10">
+        <v>200</v>
+      </c>
+      <c r="J15" s="18">
+        <v>400</v>
+      </c>
+      <c r="K15" s="19"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="28" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="17"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
+  <mergeCells count="38">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1601,30 +1291,18 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix error in uploading JOR
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F94436D-09AB-4FFD-817C-35653926D51B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -223,21 +231,72 @@
     <t>Requested By:</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>REFER TO DEPARTMENT CODE SHEET</t>
+    <t>SAMPLE REQUEST BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>SAMPLE PURPOSE BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>5 DAYS</t>
+  </si>
+  <si>
+    <t>Sample scope of work 1</t>
+  </si>
+  <si>
+    <t>Sample scope of work 2</t>
+  </si>
+  <si>
+    <t>Sample scope of work 3</t>
+  </si>
+  <si>
+    <t>Sample scope of work 4</t>
+  </si>
+  <si>
+    <t>Sample scope of work 5</t>
+  </si>
+  <si>
+    <t>lot/s</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>bot/s</t>
+  </si>
+  <si>
+    <t>roll/s</t>
+  </si>
+  <si>
+    <t>box/s</t>
+  </si>
+  <si>
+    <t>Sample note 1</t>
+  </si>
+  <si>
+    <t>Sample note 2</t>
+  </si>
+  <si>
+    <t>Sample note 3</t>
+  </si>
+  <si>
+    <t>Sample note 4</t>
+  </si>
+  <si>
+    <t>Sample note 5</t>
+  </si>
+  <si>
+    <t>BCD-ADMIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +329,14 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -277,8 +344,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,40 +523,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,24 +590,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -572,7 +635,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -869,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:K11"/>
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,14 +966,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -918,14 +981,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -933,14 +996,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -948,142 +1011,154 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="I7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="28">
+        <v>44306</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="I8" s="28">
+        <v>44313</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+        <v>26</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+      <c r="I9" s="28">
+        <v>44306</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="15">
+        <v>254655</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="C12" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="32"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1093,142 +1168,228 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="32"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="G14" s="13">
+        <v>5</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="10">
+        <v>150</v>
+      </c>
+      <c r="J14" s="18">
+        <v>750</v>
+      </c>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="26"/>
+      <c r="G15" s="13">
+        <v>2</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="10">
+        <v>415</v>
+      </c>
+      <c r="J15" s="18">
+        <v>830</v>
+      </c>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="13">
+        <v>6</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="10">
+        <v>250.25</v>
+      </c>
+      <c r="J16" s="18">
+        <v>1501.5</v>
+      </c>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="18"/>
+      <c r="A17" s="10">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="10">
+        <v>8</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="10">
+        <v>15</v>
+      </c>
+      <c r="J17" s="18">
+        <v>120</v>
+      </c>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="18"/>
+      <c r="A18" s="10">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="10">
+        <v>12</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="10">
+        <v>80.75</v>
+      </c>
+      <c r="J18" s="18">
+        <v>969</v>
+      </c>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="18"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="A20" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="18"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="B21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="18"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
+  <mergeCells count="44">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
@@ -1244,7 +1405,37 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="J24:K24"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1252,7 +1443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fix insertion of notes in upload JOR
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -246,28 +246,10 @@
     <t>Sample scope of work 2</t>
   </si>
   <si>
-    <t>Sample scope of work 3</t>
-  </si>
-  <si>
-    <t>Sample scope of work 4</t>
-  </si>
-  <si>
-    <t>Sample scope of work 5</t>
-  </si>
-  <si>
     <t>lot/s</t>
   </si>
   <si>
     <t>pc/s</t>
-  </si>
-  <si>
-    <t>bot/s</t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t>box/s</t>
   </si>
   <si>
     <t>Sample note 1</t>
@@ -514,6 +496,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,58 +508,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,6 +554,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -635,7 +617,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -933,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,14 +948,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -981,14 +963,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -996,14 +978,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -1011,154 +993,152 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="28">
+      <c r="B8" s="15"/>
+      <c r="C8" s="19">
         <v>44306</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="19">
         <v>44313</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="19">
         <v>44306</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="30"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="15">
-        <v>254655</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="16">
         <v>1</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="37"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1168,228 +1148,176 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="13">
         <v>5</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I14" s="10">
         <v>150</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="25">
         <v>750</v>
       </c>
-      <c r="K14" s="19"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="13">
         <v>2</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I15" s="10">
         <v>415</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="25">
         <v>830</v>
       </c>
-      <c r="K15" s="19"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="13">
-        <v>6</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="10">
-        <v>250.25</v>
-      </c>
-      <c r="J16" s="18">
-        <v>1501.5</v>
-      </c>
-      <c r="K16" s="19"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>4</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="10">
-        <v>8</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="10">
-        <v>15</v>
-      </c>
-      <c r="J17" s="18">
-        <v>120</v>
-      </c>
-      <c r="K17" s="19"/>
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>5</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="10">
-        <v>12</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" s="10">
-        <v>80.75</v>
-      </c>
-      <c r="J18" s="18">
-        <v>969</v>
-      </c>
-      <c r="K18" s="19"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="B19" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="17"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
+      <c r="B21" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="17"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="38">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
@@ -1405,35 +1333,6 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add JOR and JOI Report
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -246,10 +246,28 @@
     <t>Sample scope of work 2</t>
   </si>
   <si>
+    <t>Sample scope of work 3</t>
+  </si>
+  <si>
+    <t>Sample scope of work 4</t>
+  </si>
+  <si>
+    <t>Sample scope of work 5</t>
+  </si>
+  <si>
     <t>lot/s</t>
   </si>
   <si>
     <t>pc/s</t>
+  </si>
+  <si>
+    <t>bot/s</t>
+  </si>
+  <si>
+    <t>roll/s</t>
+  </si>
+  <si>
+    <t>box/s</t>
   </si>
   <si>
     <t>Sample note 1</t>
@@ -496,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,37 +523,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -554,24 +590,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -617,7 +635,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -915,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD18"/>
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,14 +966,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -963,14 +981,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -978,14 +996,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -993,152 +1011,152 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="19">
+      <c r="B8" s="26"/>
+      <c r="C8" s="28">
         <v>44306</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="28">
         <v>44313</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="28">
         <v>44306</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="15">
         <v>1</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1148,176 +1166,228 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="31"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="13">
         <v>5</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I14" s="10">
         <v>150</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="18">
         <v>750</v>
       </c>
-      <c r="K14" s="26"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="13">
         <v>2</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I15" s="10">
         <v>415</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="18">
         <v>830</v>
       </c>
-      <c r="K15" s="26"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="18"/>
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="13">
+        <v>6</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="10">
+        <v>250.25</v>
+      </c>
+      <c r="J16" s="18">
+        <v>1501.5</v>
+      </c>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="10">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="10">
+        <v>8</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="10">
+        <v>15</v>
+      </c>
+      <c r="J17" s="18">
+        <v>120</v>
+      </c>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="18"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="10">
+        <v>12</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="10">
+        <v>80.75</v>
+      </c>
+      <c r="J18" s="18">
+        <v>969</v>
+      </c>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="18"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="A20" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="18"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="B21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="18"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
+  <mergeCells count="44">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
@@ -1333,6 +1403,35 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
jo no series and fixed errors
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,37 +219,34 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Requested By:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bacolod</t>
-  </si>
-  <si>
-    <t>Bago Site ter</t>
-  </si>
-  <si>
-    <t>Retrofitting</t>
-  </si>
-  <si>
-    <t>TEST 1</t>
-  </si>
-  <si>
-    <t>TEST 2</t>
-  </si>
-  <si>
-    <t>TEST 3</t>
-  </si>
-  <si>
-    <t>Note 1</t>
-  </si>
-  <si>
-    <t>Note 2</t>
-  </si>
-  <si>
-    <t>Note 3</t>
-  </si>
-  <si>
-    <t>CENJO-EM029-369</t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t>Sample only</t>
+  </si>
+  <si>
+    <t>sample2021</t>
   </si>
 </sst>
 </file>
@@ -260,7 +257,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +304,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +352,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -448,11 +485,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,54 +699,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,57 +791,65 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -916,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,14 +1221,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -964,14 +1236,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -979,14 +1251,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -994,146 +1266,142 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="31"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="29">
-        <v>44353</v>
-      </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="42">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="31"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="17" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="33"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="51"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1143,170 +1411,203 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="33"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="26">
+        <v>10</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="13">
-        <v>10</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15">
-        <v>10000</v>
-      </c>
-      <c r="J14" s="26">
-        <f>G14*I14</f>
-        <v>100000</v>
-      </c>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="13">
-        <v>5</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15">
-        <v>200</v>
-      </c>
-      <c r="J15" s="26">
-        <f t="shared" ref="J15:J16" si="0">G15*I15</f>
-        <v>1000</v>
-      </c>
-      <c r="K15" s="27"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="24" t="s">
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="13">
-        <v>5</v>
-      </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15">
-        <v>550</v>
-      </c>
-      <c r="J16" s="26">
-        <f t="shared" si="0"/>
-        <v>2750</v>
-      </c>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="35" t="s">
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="19"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
+  <mergeCells count="41">
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1318,21 +1619,12 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1345,7 +1637,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update multiple rfd function
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,34 +219,37 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Requested By:</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>junjun</t>
-  </si>
-  <si>
-    <t>Cenjo-1001</t>
-  </si>
-  <si>
-    <t>wanders</t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t>Sample only</t>
+  </si>
+  <si>
+    <t>again</t>
+  </si>
+  <si>
+    <t>try</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,8 +307,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +355,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -445,11 +488,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,18 +702,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -488,39 +807,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -541,18 +839,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -593,7 +887,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -891,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,14 +1218,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -939,14 +1233,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -954,14 +1248,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -969,149 +1263,139 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="43"/>
+      <c r="E7" s="40"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="25">
-        <v>44362</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="51">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="25">
-        <v>44362</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="25">
-        <v>44362</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="40"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="40"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="29"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
@@ -1127,168 +1411,202 @@
       </c>
       <c r="K13" s="29"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="13">
-        <v>1</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>70</v>
+      <c r="B14" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="24">
+        <v>10</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="I14" s="10">
-        <v>22</v>
-      </c>
-      <c r="J14" s="22">
-        <v>22</v>
-      </c>
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2</v>
       </c>
-      <c r="B15" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="13">
-        <v>1</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>70</v>
+      <c r="B15" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="I15" s="10">
-        <v>22</v>
-      </c>
-      <c r="J15" s="22">
-        <v>22</v>
-      </c>
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="13">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>70</v>
+        <v>2</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="15">
+        <v>2</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="I16" s="10">
-        <v>22</v>
-      </c>
-      <c r="J16" s="22">
-        <v>22</v>
-      </c>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="18"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="18"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="41">
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1300,21 +1618,30 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C12:K12"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
additional features and fixed errors
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>try</t>
+  </si>
+  <si>
+    <t>sample general description</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -486,30 +489,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -644,19 +623,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="hair">
         <color rgb="FF000000"/>
       </top>
@@ -676,6 +642,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -684,7 +694,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -702,45 +712,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -758,34 +777,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1185,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,14 +1243,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -1233,14 +1258,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -1248,14 +1273,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -1263,140 +1288,140 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="40"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="45"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="39"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="40"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="51">
+      <c r="B8" s="50"/>
+      <c r="C8" s="56">
         <v>44273</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="53"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="40"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="45"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="53"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="40"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="45"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="40"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="45"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="40"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="45"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="40"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="45"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="54"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="29"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1406,207 +1431,217 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B15" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="24">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="24">
         <v>10</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I15" s="10">
         <v>200</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="15">
-        <v>3</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="10">
-        <v>500</v>
-      </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>2</v>
       </c>
-      <c r="B16" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>69</v>
       </c>
       <c r="I16" s="10">
+        <v>500</v>
+      </c>
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>3</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="15">
+        <v>2</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="10">
         <v>300</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="31"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="J17" s="33"/>
+      <c r="K17" s="34"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="40"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="45"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="B21" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="40"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="45"/>
     </row>
     <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
+      <c r="B22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="45"/>
     </row>
     <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="23"/>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
+  <mergeCells count="42">
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1626,22 +1661,28 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B26:F26"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
new JOR excel format
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI IT\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527CA17-67C3-4B2A-A8A1-01D996453394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="1725" yWindow="2550" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,51 +220,27 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Bacolod Office</t>
-  </si>
-  <si>
-    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
-  </si>
-  <si>
-    <t>Sample 1</t>
-  </si>
-  <si>
-    <t>Sample 2</t>
-  </si>
-  <si>
-    <t>Sample Jun</t>
-  </si>
-  <si>
-    <t>test test</t>
-  </si>
-  <si>
-    <t>Hello World</t>
-  </si>
-  <si>
-    <t>item a</t>
-  </si>
-  <si>
-    <t>item b</t>
-  </si>
-  <si>
-    <t>item c</t>
-  </si>
-  <si>
-    <t>pc</t>
+    <t>Requested By:</t>
+  </si>
+  <si>
+    <t>GENERAL DESCRIPTION</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>REFER TO DEPATMENT CODE SHEET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,50 +273,14 @@
     </font>
     <font>
       <i/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,14 +299,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -485,24 +420,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,18 +436,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,36 +465,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,70 +474,86 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
-    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,7 +594,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -990,11 +891,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,44 +910,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -1054,14 +955,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -1069,142 +970,150 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="37"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="14"/>
-      <c r="H7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="25">
-        <v>44395</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="H8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="H9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="14"/>
-      <c r="H10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="14"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="34"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1214,256 +1123,135 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>1</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="41">
-        <v>5</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="I15" s="10">
-        <v>150</v>
-      </c>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>2</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="43">
-        <v>15</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="10">
-        <v>300</v>
-      </c>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>3</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="43">
-        <v>20</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="10">
-        <v>600</v>
-      </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="44"/>
+      <c r="A14" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
       <c r="E18" s="44"/>
       <c r="F18" s="44"/>
       <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="47"/>
       <c r="G19" s="48"/>
       <c r="H19" s="48"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-    </row>
-    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B20:F20"/>
+  <mergeCells count="37">
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="C12:K12"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1475,23 +1263,31 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add other instruction function in repeat order
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$21</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -222,38 +225,59 @@
     <t>Requested By:</t>
   </si>
   <si>
-    <t>Bago</t>
-  </si>
-  <si>
-    <t>adm</t>
-  </si>
-  <si>
-    <t>1 day</t>
-  </si>
-  <si>
-    <t>Rey Carbaquil</t>
-  </si>
-  <si>
-    <t>PMS &amp; CHANGE OIL OF TOYOTA FORTUNER W/ PLATE NO. WOQ554. AS OF 09/22/21 THE ODOMETER WAS 171,193 AND AS OF 11/08/21 ODOMETER IS 176,139. TOTAL KILOMETERS TRAVELLED SINCE LAST CHANGE OIL ON 09/22/21 IS 4,946</t>
-  </si>
-  <si>
-    <t>To Provide labor, materials, tools, equipment and technical expertise for the PMS &amp; Change Oil of Toyota Fortuner w/ plate No. WOQ554</t>
-  </si>
-  <si>
-    <t>lot</t>
-  </si>
-  <si>
-    <t>1. Labor 1.1. 176,139 km Check-up
-1.1.1.  Change oil and oil Filter                                                                                                                                                                       1.1.2. Check All Fluids, Belt Charging System (Battery)                                                                                           1.1.3.  Check and Clean engine air filter                                                                                                                                                                                                                            1.1.4.  Check lights                                                                                                                                                          1.1.5. Check and Clean cabin air filter                                                                                                                                                                              1.1.6. Suspension bolt tightening                                                                                                                                                                           1.1.7.  Full Suspension Check up                                                                                                                                                                               1.1.8. Check Steering Linkages
-1.1.9.  Check/Clean/Adjust Brakes (Brake Pads &amp; Brake Shoe)                                                                                                                                                     1.1.10. Adjust Parking Brake if necessary                                                                                                                        1.1.11. Tire rotate if necessary
-1.1.12. Correct tire pressure</t>
-  </si>
-  <si>
-    <t>It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English.
-ashoxansxi0aspnciasdnci-asdnciansdciasdcas-dcna[sdcnoa]sdonco]asdcnasdncoasdncsd[</t>
-  </si>
-  <si>
-    <t>2021-ADMIN-090</t>
+    <t>Bacolod</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Supply of manpower and sevices for the following scope of work:</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Water Proofing of Concrete Wall at Switch Gear Area.</t>
+  </si>
+  <si>
+    <t>Iris Sixto / Rey D. Argawanon</t>
+  </si>
+  <si>
+    <t>Materials and equipment preparation.</t>
+  </si>
+  <si>
+    <t>Sanding and cleaning of wall surface.</t>
+  </si>
+  <si>
+    <t>Application of Thoroseal in wall surface 1st &amp; 2nd application.</t>
+  </si>
+  <si>
+    <t>Chipping, clearing of wall joints crack at 2nd floor slab  and application of  concrete grout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other necessary work activities for job completion.
+6. Hauling of materials and housekeeping.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         </t>
+  </si>
+  <si>
+    <t>CENJO-EM045-22.r4</t>
+  </si>
+  <si>
+    <t>The Contractor is requested for site visit and actual assestment of the project 2 days upon receipt of the request for quotation/proposal for further discussion w/ Cenpri in-charge personnel.</t>
+  </si>
+  <si>
+    <t>The contractor is required to accomplish all Health Data provided by CENPRI and follow company protocol within 24- hours before the scheduled site visit.</t>
+  </si>
+  <si>
+    <t>The Contractor and its personnel is required to undergo Company Safety Oreintation 1-day before the project start date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Contractor will provide the necessary Personal Protective Equipment for its workers . </t>
+  </si>
+  <si>
+    <t>Workmanship is subject for evaluation and approval of company representative .</t>
+  </si>
+  <si>
+    <t>Hauling of materials and housekeeping.</t>
   </si>
 </sst>
 </file>
@@ -264,7 +288,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,12 +320,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -324,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -444,140 +527,234 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 5 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -609,7 +786,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -916,238 +1093,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="45" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="45" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="40" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="43"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
+    </row>
+    <row r="7" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="22">
-        <v>44524</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="36">
+        <v>44662</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="22">
-        <v>44526</v>
-      </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="22">
-        <v>44525</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="I9" s="54"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="56"/>
+    </row>
+    <row r="10" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="11" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="B11" s="57"/>
+      <c r="C11" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="50"/>
+    </row>
+    <row r="12" spans="1:36" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="17"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="29"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1157,171 +1360,249 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="15" spans="1:11" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="K13" s="65"/>
+    </row>
+    <row r="14" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
         <v>1</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="26">
+        <v>1</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>2</v>
+      </c>
+      <c r="B16" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="14">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>3</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>4</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>5</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>6</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" spans="1:11" s="19" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="27"/>
+      <c r="B21" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="69"/>
+    </row>
+    <row r="22" spans="1:11" s="19" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="69"/>
+    </row>
+    <row r="23" spans="1:11" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="1:11" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="34">
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="B21:K21"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1331,7 +1612,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add disable button if saving in deliver_po
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E53A10-9CB1-45B6-AEAE-D46BC224FF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -223,39 +222,40 @@
     <t>Requested By:</t>
   </si>
   <si>
-    <t>asdasdasd</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>sdfsdfs</t>
-  </si>
-  <si>
-    <t>Sample Description</t>
-  </si>
-  <si>
-    <t>Item 1</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Item 2</t>
-  </si>
-  <si>
-    <t>Item 3</t>
+    <t>GENERAL DESCRIPTION</t>
+  </si>
+  <si>
+    <t>REFER TO DEPARTMENT CODE SHEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Labor
+A. Replace advise parts
+a.1. Rack End
+a.2. Tie Rod End
+B. Wheel Alignment</t>
+  </si>
+  <si>
+    <t>bacolod</t>
+  </si>
+  <si>
+    <t>ADM 1001</t>
+  </si>
+  <si>
+    <t>Stephine</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +294,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -445,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -522,6 +516,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -609,7 +609,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -906,25 +906,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B21" sqref="B21:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -937,7 +937,7 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
       <c r="C2" s="29" t="s">
@@ -952,7 +952,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="32" t="s">
@@ -967,7 +967,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="32" t="s">
@@ -982,7 +982,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="25" t="s">
@@ -997,7 +997,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
@@ -1012,15 +1012,15 @@
       <c r="J6" s="27"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="34"/>
+        <v>68</v>
+      </c>
+      <c r="D7" s="36"/>
       <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1028,31 +1028,31 @@
         <v>55</v>
       </c>
       <c r="I7" s="20"/>
-      <c r="J7" s="34"/>
+      <c r="J7" s="36"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="33">
-        <v>44750</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+        <v>44841</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11" t="s">
         <v>58</v>
       </c>
       <c r="I8" s="33">
-        <v>44750</v>
-      </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44841</v>
+      </c>
+      <c r="J8" s="34"/>
+      <c r="K8" s="35"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>56</v>
       </c>
@@ -1060,26 +1060,28 @@
       <c r="C9" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="11" t="s">
         <v>59</v>
       </c>
       <c r="I9" s="33">
-        <v>44750</v>
-      </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44841</v>
+      </c>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="30"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="36"/>
       <c r="E10" s="21"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1087,54 +1089,54 @@
         <v>9</v>
       </c>
       <c r="I10" s="20"/>
-      <c r="J10" s="34"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="21"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="34"/>
+        <v>70</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="21"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1144,90 +1146,72 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" s="40"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>1</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="14">
-        <v>10</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>70</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="23"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>2</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>71</v>
-      </c>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="14">
-        <v>10</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>70</v>
-      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
-        <v>3</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>72</v>
-      </c>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="14">
-        <v>10</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>70</v>
-      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="22"/>
       <c r="C18" s="18"/>
@@ -1240,7 +1224,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>63</v>
       </c>
@@ -1255,7 +1239,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1268,7 +1252,7 @@
       <c r="J20" s="20"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1321,7 +1305,6 @@
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="J17:K17"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1329,19 +1312,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1357,7 +1340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1365,7 +1348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1356,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1381,7 +1364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1389,7 +1372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1380,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1405,7 +1388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1413,7 +1396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1421,7 +1404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1429,7 +1412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1437,7 +1420,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1445,7 +1428,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1453,7 +1436,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1461,7 +1444,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1469,7 +1452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1477,7 +1460,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1485,7 +1468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1501,7 +1484,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1509,7 +1492,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
upgrade import and export to php 8
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,32 +219,40 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Requested By:</t>
-  </si>
-  <si>
-    <t>GENERAL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>REFER TO DEPARTMENT CODE SHEET</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Labor
-A. Replace advise parts
-a.1. Rack End
-a.2. Tie Rod End
-B. Wheel Alignment</t>
-  </si>
-  <si>
-    <t>bacolod</t>
-  </si>
-  <si>
-    <t>ADM 1001</t>
-  </si>
-  <si>
-    <t>Stephine</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>Bacolod Office</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT Office Renovation</t>
+  </si>
+  <si>
+    <t>Manpower: Breakdown of manpower personnel, to note level of expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPEs: Contractor to provide own PPEs and attend to safety briefing first day of work. before conducting </t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t>Sample only</t>
+  </si>
+  <si>
+    <t>again</t>
+  </si>
+  <si>
+    <t>sample general description</t>
+  </si>
+  <si>
+    <t>Sample 3</t>
   </si>
 </sst>
 </file>
@@ -255,7 +263,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,14 +296,50 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +358,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -435,11 +491,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,45 +706,136 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,68 +853,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -907,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,44 +1228,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -970,14 +1273,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -985,157 +1288,139 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="27"/>
+      <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="33">
-        <v>44841</v>
-      </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="52">
+        <v>44273</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="33">
-        <v>44841</v>
-      </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="H9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="65"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="27"/>
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="33">
-        <v>44841</v>
-      </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="21"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="50"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="40"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
@@ -1146,141 +1431,208 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="38" t="s">
         <v>61</v>
       </c>
       <c r="K13" s="40"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A14" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>1</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="24">
+        <v>5</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="10">
+        <v>200</v>
+      </c>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>2</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="15">
+        <v>2</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="10">
+        <v>500</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="14">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="21"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
+  <mergeCells count="42">
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1292,21 +1644,40 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix error when saving total price in po and pod
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kervic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiji\Desktop\ADMIN JOR &amp; PR\ADMIN JO\ADMIN JO 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -44,6 +52,9 @@
     <t xml:space="preserve">JO Request to: </t>
   </si>
   <si>
+    <t>Bacolod</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Duration:</t>
   </si>
   <si>
@@ -56,7 +67,7 @@
     <t xml:space="preserve">                      Department:</t>
   </si>
   <si>
-    <t>Operations</t>
+    <t>ADMIN</t>
   </si>
   <si>
     <t xml:space="preserve">      Delivery Date:</t>
@@ -71,9 +82,6 @@
     <t>Requested By:</t>
   </si>
   <si>
-    <t>Godfrey S. E. Samano</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Purpose:</t>
   </si>
   <si>
@@ -95,40 +103,38 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>Fabrication of Replacement Parts for Fuel Module No. 4 and Fuel Pump No. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply of manpower/labor and technical expertise for the Fabrication of Fuel Module No. 4 and Fuel Pump No. 1 Replacement Parts.                 </t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>As Per Drawing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scope of works include but not limited to:
-1. Fabrication of Rubber Spider Coupling Insert         
-Material: Viton      
-2. Other work activities seen necessary for the job completion             
-       </t>
-  </si>
-  <si>
-    <t>CENJO-EM023-2024</t>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>Rey Carbaquil</t>
+  </si>
+  <si>
+    <t>Replacement of expired window tint of Ford Everest with plate no. NBR 8308</t>
+  </si>
+  <si>
+    <t>To provide  labor, tools, equipment and technical expertise for the replacement of expired window tint of Ford Everest with plate no. NBR 8308</t>
+  </si>
+  <si>
+    <t>JOR-ADM-023-2024</t>
+  </si>
+  <si>
+    <t>Labor
+removal and installation</t>
+  </si>
+  <si>
+    <t>Materials
+full car tint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,29 +166,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -192,21 +175,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -241,6 +209,48 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -250,10 +260,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -261,18 +271,7 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -282,7 +281,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -290,7 +289,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -311,7 +310,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -321,7 +320,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -346,6 +345,67 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -376,172 +436,159 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -566,22 +613,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03D51852-5E37-4F17-B4FC-3529E33CFE05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C6F9F4-80D9-4469-9C20-7C9BA33AC016}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -603,8 +650,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="381000"/>
-          <a:ext cx="1200150" cy="304800"/>
+          <a:off x="361950" y="381000"/>
+          <a:ext cx="1200150" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -616,22 +663,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{449B55C9-235A-494C-B098-099C4E81B07B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4062CAC3-A5B2-4E57-8DD1-9C4A36C9F666}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -653,8 +700,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="381000"/>
-          <a:ext cx="1200150" cy="304800"/>
+          <a:off x="361950" y="381000"/>
+          <a:ext cx="1200150" cy="314325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -965,304 +1012,314 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="1.42578125" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="56" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="57" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="7"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="58" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="H7" s="11" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="H7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38">
-        <v>45358</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="H8" s="11" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="41"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="43"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34">
+        <v>45471</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="H8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="44" t="s">
+      <c r="I8" s="34"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
-      <c r="H9" s="11" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="H9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="34"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="31" t="s">
+      <c r="A10" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="H10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="28">
+        <v>1</v>
+      </c>
+      <c r="J10" s="29"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="43"/>
+    </row>
+    <row r="12" spans="1:11" s="15" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="56"/>
+    </row>
+    <row r="14" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>1</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="19">
+        <v>1</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>2</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="32"/>
-      <c r="H10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="31">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="19">
         <v>1</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
-    </row>
-    <row r="15" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <v>1</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="16">
-        <v>2</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-    </row>
-    <row r="16" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="H16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
       <c r="I16" s="20"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="I8:K8"/>
@@ -1274,18 +1331,11 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="88" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="12" max="1048575" man="1"/>
+    <brk id="11" max="1048575" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
required description in rfd of joi and jod and fixed draft of joi vat has wrong computation
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Requested By:</t>
   </si>
   <si>
-    <t>2 dyas</t>
-  </si>
-  <si>
     <t>Glenn Paul Toledo</t>
   </si>
   <si>
@@ -246,13 +243,10 @@
     <t>Item 10</t>
   </si>
   <si>
-    <t>Item 11</t>
-  </si>
-  <si>
-    <t>Item 12</t>
-  </si>
-  <si>
-    <t>GPT00020</t>
+    <t>GPT00030</t>
+  </si>
+  <si>
+    <t>2 days</t>
   </si>
 </sst>
 </file>
@@ -476,97 +470,97 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:K12"/>
+      <selection activeCell="I7" sqref="I7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,14 +936,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="5"/>
@@ -957,14 +951,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -972,14 +966,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -987,160 +981,160 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="36"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="33">
+      <c r="B8" s="36"/>
+      <c r="C8" s="22">
         <v>45491</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="22">
         <v>45491</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="35"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="22">
         <v>45491</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="21"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="21"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
+      <c r="C12" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1150,32 +1144,32 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="38"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44"/>
+      <c r="A14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>72</v>
+      <c r="B15" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -1185,124 +1179,93 @@
         <v>1</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="13">
         <v>5000</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="19">
         <v>5000</v>
       </c>
-      <c r="K15" s="24"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <v>2</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="14">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="13">
-        <v>6000</v>
-      </c>
-      <c r="J16" s="23">
-        <v>6000</v>
-      </c>
-      <c r="K16" s="24"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <v>3</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>74</v>
+      <c r="A17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="14">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="13">
-        <v>7000</v>
-      </c>
-      <c r="J17" s="23">
-        <v>7000</v>
-      </c>
-      <c r="K17" s="24"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>69</v>
-      </c>
+      <c r="A19" s="16"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="21"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="33">
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="A10:B10"/>
@@ -1317,29 +1280,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>

</xml_diff>